<commit_message>
final commit before turning in
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Git\CourseRegistrationPOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A9828C-EB5F-4CC5-9FA8-42F0FC15E738}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A3010A-2A94-43F4-86D8-F5B69628C11B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{69547CC7-FCD1-46E6-BB03-ADC52D6C46F5}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -459,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECC314D-CC49-4A88-A6B6-800893CEF42F}">
-  <dimension ref="A1:H126"/>
+  <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,8 +524,8 @@
         <v>7.6388888888888895E-2</v>
       </c>
       <c r="G3" s="7">
-        <f>SUM(E3:E126)</f>
-        <v>11.648611111111114</v>
+        <f>SUM(E3:E128)</f>
+        <v>11.845833333333337</v>
       </c>
       <c r="H3" s="7"/>
     </row>
@@ -2264,7 +2264,7 @@
         <v>0.65625</v>
       </c>
       <c r="E100" s="5">
-        <f t="shared" ref="E100:E125" si="3">D100-C100</f>
+        <f t="shared" ref="E100:E128" si="3">D100-C100</f>
         <v>0.17708333333333331</v>
       </c>
     </row>
@@ -2731,6 +2731,42 @@
       </c>
       <c r="E126" s="5">
         <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" s="1">
+        <v>43441</v>
+      </c>
+      <c r="C127" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D127" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E127" s="5">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128" s="1">
+        <v>43441</v>
+      </c>
+      <c r="C128" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D128" s="2">
+        <v>0.59305555555555556</v>
+      </c>
+      <c r="E128" s="5">
+        <f t="shared" si="3"/>
+        <v>0.11388888888888887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>